<commit_message>
Initial Glider Design v5.2
- Python
- Add roll-in time as objective
</commit_message>
<xml_diff>
--- a/01_Initial_Glider_Design/results/Nausicaa_v_5_1/nausicaa_results.xlsx
+++ b/01_Initial_Glider_Design/results/Nausicaa_v_5_1/nausicaa_results.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.188767559013193</v>
+        <v>5.141061488777358</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.00000009983609</v>
+        <v>10.00000009984927</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>65.00000064773005</v>
+        <v>65.00000064741765</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.279770101643094</v>
+        <v>1.256345602973553</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.366201640517977</v>
+        <v>2.366201640490309</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08221959477081109</v>
+        <v>0.082776784967591</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8.911488183922959</v>
+        <v>8.087660995730328</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.377735120416266</v>
+        <v>1.504116959379239</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.290956453270083</v>
+        <v>1.419258604085065</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.08677866714618299</v>
+        <v>-0.08485835529417374</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03999999039489697</v>
+        <v>0.03999999054947855</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3999999900708682</v>
+        <v>0.3999999900529826</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02595821735867678</v>
+        <v>0.01999999000524019</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49622.03744639546</v>
+        <v>49463.23004825977</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.1192494439132623</v>
+        <v>-0.1015359300736017</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.8116548750733799</v>
+        <v>0.8056713411417376</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.8024143396509142</v>
+        <v>0.8114614932495552</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.015407343537959</v>
+        <v>2.053750222914737</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1396938327061588</v>
+        <v>0.1405388941806902</v>
       </c>
     </row>
     <row r="21">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1120923345242177</v>
+        <v>0.1140419009315041</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.8116548750733799</v>
+        <v>0.8056713411417376</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1756915437222578</v>
+        <v>0.1784068470628501</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04392288593056445</v>
+        <v>0.04460171176571253</v>
       </c>
     </row>
     <row r="26">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.007716879633877508</v>
+        <v>0.007957250769726797</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.8116548750733799</v>
+        <v>0.8056713411417376</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.07584972789047741</v>
+        <v>0.06778242641157563</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0379248639452387</v>
+        <v>0.03389121320578781</v>
       </c>
     </row>
     <row r="31">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.002876590610529733</v>
+        <v>0.002297228665120333</v>
       </c>
     </row>
     <row r="33">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-1.782394647514879e-17</v>
+        <v>1.873081839836726e-16</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-9.12868733416811e-15</v>
+        <v>1.051024499184463e-14</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-3.131824590131445</v>
+        <v>10.00580694703766</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.3373643059049394</v>
+        <v>0.2288781246149695</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2.076364045088156</v>
+        <v>1.363862811138331</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.362726895657417</v>
+        <v>4.956629328400594</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-36.47434858649417</v>
+        <v>-40.62063333904845</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.4864628843528964</v>
+        <v>0.4866281482450332</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1.061629305784189</v>
+        <v>1.065901365063418</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.007575611267905819</v>
+        <v>0.007249436612822757</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.053955611263649</v>
+        <v>1.057650766723981</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>9.808325263351997e-05</v>
+        <v>0.001001161726613871</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>3.488338179462102e-10</v>
+        <v>3.425414303793734e-10</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.02549194692891806</v>
+        <v>0.03284266895617405</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-2.844519349068593e-18</v>
+        <v>1.657703153232167e-20</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.003076769045250621</v>
+        <v>0.003182731310834771</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.001859155498363363</v>
+        <v>0.001945924981551996</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.002125264973090249</v>
+        <v>0.001961788972003531</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.003980573522275391</v>
+        <v>0.003903935295313687</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1.860566726111062e-21</v>
+        <v>-1.02986929694753e-21</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-8.50962934796365e-06</v>
+        <v>-4.487751216942977e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2.764330990684678e-21</v>
+        <v>-2.741783423357421e-21</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.03214082109098478</v>
+        <v>0.03289764425245234</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.000613002378438925</v>
+        <v>0.0006418656542215293</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.0001973020764126254</v>
+        <v>0.0001408059179581332</v>
       </c>
     </row>
     <row r="61">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.008378138870879778</v>
+        <v>0.008164865440938052</v>
       </c>
     </row>
     <row r="66">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-9.999298427849666e-09</v>
+        <v>-9.999282099889604e-09</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.006090340353393414</v>
+        <v>0.006131613701303038</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.03492345817653969</v>
+        <v>-0.03513472354517255</v>
       </c>
     </row>
     <row r="70">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.03492345817653969</v>
+        <v>-0.03513472354517255</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.4009589855179244</v>
+        <v>0.4054701244248722</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.01410975023840067</v>
+        <v>0.0145401841658935</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.7677319891428154</v>
+        <v>0.7610696293760251</v>
       </c>
     </row>
     <row r="76">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.7677319891428154</v>
+        <v>0.7610696293760251</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.08784577186112891</v>
+        <v>0.08920342353142506</v>
       </c>
     </row>
     <row r="80">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.7737300111281411</v>
+        <v>0.7717801279359497</v>
       </c>
     </row>
     <row r="82">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.7737300111281411</v>
+        <v>0.7717801279359497</v>
       </c>
     </row>
     <row r="85">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.07584972789047741</v>
+        <v>0.06778242641157563</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.1205004768104272</v>
+        <v>-0.09968772864805175</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-1.318836058167139e-17</v>
+        <v>-5.16967716399672e-18</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>1.916711713627863</v>
+        <v>1.933514829472097</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>4.794372147685108e-19</v>
+        <v>1.393605914562689e-19</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-1.713039432527097e-17</v>
+        <v>2.369068483054626e-14</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-8.862858618694539e-18</v>
+        <v>-3.743027284758309e-18</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.1205004768104272</v>
+        <v>0.09968772864805175</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-0.2141636957052923</v>
+        <v>-0.2375780819255464</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-4.794372147685108e-19</v>
+        <v>-1.393605914562689e-19</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>1.066865777223046e-18</v>
+        <v>5.127264824914205e-19</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>1.908517243702988</v>
+        <v>1.921450986629662</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-1.318836058167139e-17</v>
+        <v>-5.16967716399672e-18</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.2141636957052923</v>
+        <v>0.2375780819255464</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-4.794372147685108e-19</v>
+        <v>-1.393605914562689e-19</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-1.713039432527097e-17</v>
+        <v>2.369068483054626e-14</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>8.862858618694539e-18</v>
+        <v>3.743027284758309e-18</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1.032490223535596</v>
+        <v>1.04076690245188</v>
       </c>
     </row>
     <row r="104">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-7.13478141733628e-18</v>
+        <v>-2.80019054666946e-18</v>
       </c>
     </row>
     <row r="105">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.1158605838021857</v>
+        <v>0.1286857724379556</v>
       </c>
     </row>
     <row r="106">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-3.232383791722652e-19</v>
+        <v>-9.302426065963594e-20</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-6.634069041855081e-17</v>
+        <v>9.13072462700741e-14</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>5.975372721374994e-18</v>
+        <v>2.498499340129082e-18</v>
       </c>
     </row>
     <row r="109">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1.856413828678073</v>
+        <v>1.85433148830393</v>
       </c>
     </row>
     <row r="110">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.06846880417355733</v>
+        <v>0.0687012905396126</v>
       </c>
     </row>
     <row r="111">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.03874544324876744</v>
+        <v>0.05210876440430913</v>
       </c>
     </row>
     <row r="114">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-8.673617379884035e-19</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="115">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.8019181245611473</v>
+        <v>0.810940416261092</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.8000429494654813</v>
+        <v>0.799863895922665</v>
       </c>
     </row>
     <row r="117">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.05008571009645443</v>
+        <v>0.06518784432642251</v>
       </c>
     </row>
     <row r="118">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.006158163896558258</v>
+        <v>0.02827084386690126</v>
       </c>
     </row>
     <row r="119">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-5.421010862427522e-20</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.03792203369293522</v>
+        <v>-0.05133653947947021</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-3.388131789017201e-21</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="123">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.1756915437222578</v>
+        <v>0.1784068470628501</v>
       </c>
     </row>
     <row r="124">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>2.710505431213761e-20</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>0.001342019009670646</v>
+        <v>0.001118499802978656</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-1.318836058167139e-17</v>
+        <v>-5.16967716399672e-18</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-4.188157959616214e-19</v>
+        <v>-1.393963855822461e-19</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.0001299646828314886</v>
+        <v>-0.0001109254283923663</v>
       </c>
     </row>
     <row r="130">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>9.730300033035297e-18</v>
+        <v>3.743045881230322e-18</v>
       </c>
     </row>
     <row r="131">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.07584972789047741</v>
+        <v>0.06778242641157563</v>
       </c>
     </row>
     <row r="132">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.002017704928461105</v>
+        <v>0.001931653999308799</v>
       </c>
     </row>
     <row r="134">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.001536816722874918</v>
+        <v>0.001479730226180829</v>
       </c>
     </row>
     <row r="135">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-6.411310182614223e-21</v>
+        <v>3.579412597724902e-23</v>
       </c>
     </row>
     <row r="137">
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>-0.0006934448730007532</v>
+        <v>-0.0006612994964228587</v>
       </c>
     </row>
     <row r="138">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>3.308455436662653e-21</v>
+        <v>-1.859647201169946e-23</v>
       </c>
     </row>
     <row r="139">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.07750580380266114</v>
+        <v>0.09957036443567334</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.1366578919026311</v>
+        <v>0.1380077174898731</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>3.995925788714763</v>
+        <v>4.021942757509349</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.6545847842128417</v>
+        <v>0.7196226212683181</v>
       </c>
     </row>
     <row r="145">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>2.710736992696813e-22</v>
+        <v>1.044407914869513e-22</v>
       </c>
     </row>
     <row r="146">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>1.123452428669068e-19</v>
+        <v>7.352052803835053e-20</v>
       </c>
     </row>
     <row r="147">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-0.1598369931673116</v>
+        <v>-0.1608776722909176</v>
       </c>
     </row>
     <row r="148">
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>3.357080992817456e-14</v>
+        <v>1.283184935960032e-20</v>
       </c>
     </row>
     <row r="149">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.03107969889539075</v>
+        <v>0.03846422339523582</v>
       </c>
     </row>
     <row r="150">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-5.356868305583017e-06</v>
+        <v>-5.438672171990259e-06</v>
       </c>
     </row>
     <row r="151">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-5.248646751991539e-07</v>
+        <v>-6.659143239353572e-07</v>
       </c>
     </row>
     <row r="152">
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.1303372947511667</v>
+        <v>0.1396629135786665</v>
       </c>
     </row>
     <row r="153">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.0249999900006403</v>
+        <v>-0.02499999013591874</v>
       </c>
     </row>
     <row r="154">
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>6.628917143426543e-07</v>
+        <v>6.800997353113348e-07</v>
       </c>
     </row>
     <row r="155">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.02999999001058695</v>
+        <v>0.03217912957886197</v>
       </c>
     </row>
     <row r="156">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>-0.15920133076905</v>
+        <v>-0.1541226740289295</v>
       </c>
     </row>
     <row r="157">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.00821587771349108</v>
+        <v>-0.008244218856257035</v>
       </c>
     </row>
     <row r="158">
@@ -2012,7 +2012,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-0.001690943732965411</v>
+        <v>-0.001687347275042273</v>
       </c>
     </row>
     <row r="159">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0.07772943538876527</v>
+        <v>-0.07811761688372774</v>
       </c>
     </row>
     <row r="160">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>-0.6449211426482958</v>
+        <v>-0.6462573293105381</v>
       </c>
     </row>
     <row r="161">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>-0.0004156759886336094</v>
+        <v>-0.00121457648932765</v>
       </c>
     </row>
     <row r="162">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-0.2714076727518329</v>
+        <v>-0.2729271052266445</v>
       </c>
     </row>
     <row r="163">
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.382951487485128</v>
+        <v>0.7477096698742525</v>
       </c>
     </row>
     <row r="164">
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.5499755410149492</v>
+        <v>1.261830316836743</v>
       </c>
     </row>
     <row r="165">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-2.061854211890992e-17</v>
+        <v>-8.218579486610794e-18</v>
       </c>
     </row>
     <row r="166">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>9.733513065782946e-19</v>
+        <v>5.335777174684998e-19</v>
       </c>
     </row>
     <row r="167">
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-12.10607208972542</v>
+        <v>-16.67366636131237</v>
       </c>
     </row>
     <row r="168">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>6.040412031946941e-16</v>
+        <v>7.47333886625152e-18</v>
       </c>
     </row>
     <row r="169">
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>-0.0001431268750184955</v>
+        <v>-0.0001276918790704684</v>
       </c>
     </row>
     <row r="170">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-6.712157711585842e-05</v>
+        <v>-3.214774066395698e-05</v>
       </c>
     </row>
     <row r="171">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.1073597440598234</v>
+        <v>0.1128903331558799</v>
       </c>
     </row>
     <row r="172">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.2244197118753349</v>
+        <v>0.2225041885802361</v>
       </c>
     </row>
     <row r="173">
@@ -2162,7 +2162,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>-8.794040775672072e-05</v>
+        <v>-0.0002291904815012994</v>
       </c>
     </row>
     <row r="174">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>-0.07145586446064522</v>
+        <v>-0.07231340753291615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>